<commit_message>
Have added the changes in common, frontend and backend
</commit_message>
<xml_diff>
--- a/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
+++ b/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Have added changes in common, db, frontend, backend
</commit_message>
<xml_diff>
--- a/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
+++ b/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>0753698745</t>
   </si>
@@ -37,12 +37,6 @@
     <t>KATUNZI</t>
   </si>
   <si>
-    <t>KASHAI</t>
-  </si>
-  <si>
-    <t>1986-01-12</t>
-  </si>
-  <si>
     <t>FORM_FOUR_INDEX_NUMBER</t>
   </si>
   <si>
@@ -52,21 +46,12 @@
     <t>MIDDLE_NAME</t>
   </si>
   <si>
-    <t>PLACE_OF_BIRTH(WARD)</t>
-  </si>
-  <si>
     <t>MOBILE_PHONE_NUMBER</t>
   </si>
   <si>
-    <t>NAME_OF_INSTITUTION_OF_STUDY</t>
-  </si>
-  <si>
     <t>NATIONAL_IDENTIFICATION_NUMBER</t>
   </si>
   <si>
-    <t>1212</t>
-  </si>
-  <si>
     <t>GENDER(MALE_OR_FEMALE)</t>
   </si>
   <si>
@@ -79,24 +64,6 @@
     <t>EMPLOYEE_ID</t>
   </si>
   <si>
-    <t>GROSS_SALARY(TZS)</t>
-  </si>
-  <si>
-    <t>DATE_OF_BIRTH</t>
-  </si>
-  <si>
-    <t>ENTRY_YEAR</t>
-  </si>
-  <si>
-    <t>COMPLETION_YEAR</t>
-  </si>
-  <si>
-    <t>LEVEL_OF_STUDY</t>
-  </si>
-  <si>
-    <t>PROGRAMME_STUDIED</t>
-  </si>
-  <si>
     <t>2005</t>
   </si>
   <si>
@@ -121,29 +88,83 @@
     <t>Bachelor</t>
   </si>
   <si>
-    <t>Masters</t>
-  </si>
-  <si>
     <t>Diploma</t>
   </si>
   <si>
-    <t>Postgraduate Diploma</t>
-  </si>
-  <si>
-    <t>PhD</t>
-  </si>
-  <si>
     <t>FEMALE</t>
+  </si>
+  <si>
+    <t>LOAN_BENEFICIARY_STATUS</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>STUDY_LEVEL1</t>
+  </si>
+  <si>
+    <t>INSTITUTION_OF_STUDY1</t>
+  </si>
+  <si>
+    <t>ENTRY_YEAR1</t>
+  </si>
+  <si>
+    <t>COMPLETION_YEAR1</t>
+  </si>
+  <si>
+    <t>STUDY_LEVEL2</t>
+  </si>
+  <si>
+    <t>INSTITUTION_OF_STUDY2</t>
+  </si>
+  <si>
+    <t>ENTRY_YEAR2</t>
+  </si>
+  <si>
+    <t>COMPLETION_YEAR2</t>
+  </si>
+  <si>
+    <t>STUDY_LEVEL3</t>
+  </si>
+  <si>
+    <t>INSTITUTION_OF_STUDY3</t>
+  </si>
+  <si>
+    <t>ENTRY_YEAR3</t>
+  </si>
+  <si>
+    <t>COMPLETION_YEAR3</t>
+  </si>
+  <si>
+    <t>PROGRAMME_STUDIED1</t>
+  </si>
+  <si>
+    <t>PROGRAMME_STUDIED2</t>
+  </si>
+  <si>
+    <t>PROGRAMME_STUDIED3</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>Ardhi University</t>
+  </si>
+  <si>
+    <t>BACHELOR OF SCIENCE IN CIVIL/COMPUTER ENGINEERING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +174,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,29 +248,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AS4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,180 +580,219 @@
     <col min="3" max="3" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="26.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="4" customWidth="1"/>
     <col min="10" max="10" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="20.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="37" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="20.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="20.28515625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="20.28515625" style="4" customWidth="1"/>
+    <col min="24" max="24" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="5"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="10" t="s">
+      <c r="AP2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="AQ4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS4" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="12">
-        <v>12536</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="8">
-        <v>500000</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AH3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AH4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AI5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AI6" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R4">
-      <formula1>$AH$2:$AH$4</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z4">
+      <formula1>$AP$2:$AP$4</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2">
-      <formula1>$AI$2:$AI$6</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>$AR$2:$AR$3</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="Q2">
-      <formula1>$AJ$2:$AJ$3</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N2 S2 I2">
+      <formula1>$AQ$2:$AQ$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="X2">
+      <formula1>$AS:$AS</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Have added some changes in frontend, backend, db and common
</commit_message>
<xml_diff>
--- a/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
+++ b/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>0753698745</t>
   </si>
@@ -106,51 +106,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>STUDY_LEVEL1</t>
-  </si>
-  <si>
-    <t>INSTITUTION_OF_STUDY1</t>
-  </si>
-  <si>
-    <t>ENTRY_YEAR1</t>
-  </si>
-  <si>
-    <t>COMPLETION_YEAR1</t>
-  </si>
-  <si>
-    <t>STUDY_LEVEL2</t>
-  </si>
-  <si>
-    <t>INSTITUTION_OF_STUDY2</t>
-  </si>
-  <si>
-    <t>ENTRY_YEAR2</t>
-  </si>
-  <si>
-    <t>COMPLETION_YEAR2</t>
-  </si>
-  <si>
-    <t>STUDY_LEVEL3</t>
-  </si>
-  <si>
-    <t>INSTITUTION_OF_STUDY3</t>
-  </si>
-  <si>
-    <t>ENTRY_YEAR3</t>
-  </si>
-  <si>
-    <t>COMPLETION_YEAR3</t>
-  </si>
-  <si>
-    <t>PROGRAMME_STUDIED1</t>
-  </si>
-  <si>
-    <t>PROGRAMME_STUDIED2</t>
-  </si>
-  <si>
-    <t>PROGRAMME_STUDIED3</t>
-  </si>
-  <si>
     <t>Certificate</t>
   </si>
   <si>
@@ -158,6 +113,24 @@
   </si>
   <si>
     <t>BACHELOR OF SCIENCE IN CIVIL/COMPUTER ENGINEERING</t>
+  </si>
+  <si>
+    <t>FORM_FOUR_COMPLETION_YEAR</t>
+  </si>
+  <si>
+    <t>STUDY_LEVEL</t>
+  </si>
+  <si>
+    <t>INSTITUTION_OF_STUDY</t>
+  </si>
+  <si>
+    <t>PROGRAMME_STUDIED</t>
+  </si>
+  <si>
+    <t>ENTRY_YEAR</t>
+  </si>
+  <si>
+    <t>COMPLETION_YEAR</t>
   </si>
 </sst>
 </file>
@@ -251,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -261,10 +234,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -567,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS4"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,28 +548,23 @@
     <col min="1" max="1" width="5.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="26.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="20.28515625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="20.28515625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="20.28515625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="37" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="20.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -610,76 +575,49 @@
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="J1" s="8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -689,110 +627,99 @@
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="6">
+        <v>2004</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH3" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="5"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>27</v>
+      <c r="AI3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AP3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AP4" t="s">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG4" t="s">
         <v>22</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS4" t="s">
+      <c r="AH4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z4">
-      <formula1>$AP$2:$AP$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q4">
+      <formula1>$AG$2:$AG$4</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2">
-      <formula1>$AR$2:$AR$3</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>$AI$2:$AI$3</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N2 S2 I2">
-      <formula1>$AQ$2:$AQ$4</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>$AH$2:$AH$4</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="X2">
-      <formula1>$AS:$AS</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="O2">
+      <formula1>$AJ$2:$AJ$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Have added changes in frontend, backend, common and db
</commit_message>
<xml_diff>
--- a/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
+++ b/frontend/web/dwload/EMPLOYEES_DETAILS_TEMPLATE.xlsx
@@ -58,9 +58,6 @@
     <t>MALE</t>
   </si>
   <si>
-    <t>S0125.0065.2004</t>
-  </si>
-  <si>
     <t>EMPLOYEE_ID</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>COMPLETION_YEAR</t>
+  </si>
+  <si>
+    <t>S0125.0065</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,13 +569,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>8</v>
@@ -593,28 +593,28 @@
         <v>10</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="O1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -622,10 +622,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6">
         <v>2004</v>
@@ -646,65 +646,65 @@
         <v>0</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
-        <v>32</v>
-      </c>
       <c r="M2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="O2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AH2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AI2" t="s">
         <v>13</v>
       </c>
       <c r="AJ2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AG3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AH3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI3" t="s">
         <v>24</v>
       </c>
-      <c r="AI3" t="s">
-        <v>25</v>
-      </c>
       <c r="AJ3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AG4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AH4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AJ4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>